<commit_message>
Added excel directly again
</commit_message>
<xml_diff>
--- a/Summarized Trials.xlsx
+++ b/Summarized Trials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e54ee0e16b764741/University/Fa2023/ECE 718 - Compiler Design for High Performance/Project/GemmCUDA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="526" documentId="13_ncr:1_{3C733FE7-E8A4-42C6-AC06-D019A0768725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F1F7CEC-6BA5-46A6-A282-40DD598BC6E9}"/>
+  <xr:revisionPtr revIDLastSave="567" documentId="13_ncr:1_{3C733FE7-E8A4-42C6-AC06-D019A0768725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9B52203-E574-4916-A107-CF35669F45D6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Trials" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="419">
   <si>
     <t>Trial Name</t>
   </si>
@@ -1315,6 +1315,21 @@
   </si>
   <si>
     <t>Threads Per Block</t>
+  </si>
+  <si>
+    <t>Loop Reordering JIT</t>
+  </si>
+  <si>
+    <t>Naïve</t>
+  </si>
+  <si>
+    <t>Naïve JIT</t>
+  </si>
+  <si>
+    <t>Naïve CUDA</t>
+  </si>
+  <si>
+    <t>CUDA Vectorization</t>
   </si>
 </sst>
 </file>
@@ -1985,7 +2000,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive Time</c:v>
+                  <c:v>Naïve</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2090,7 +2105,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive Time Numba</c:v>
+                  <c:v>Naïve JIT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2195,7 +2210,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ikj Time Numba</c:v>
+                  <c:v>Loop Reordering JIT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2300,7 +2315,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CUDA Time naive</c:v>
+                  <c:v>Naïve CUDA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2428,6 +2443,79 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Square</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Array Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2491,6 +2579,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2630,6 +2778,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CUDA Shared Memory Caching</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3072,6 +3245,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CUDA T Shared Memory Caching</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3588,7 +3786,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CUDA Time naive</c:v>
+                  <c:v>Naïve CUDA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3693,7 +3891,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CUDA Time Global Memory Coalescing</c:v>
+                  <c:v>CUDA Global Memory Coalescing</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3798,7 +3996,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CUDA Time Shared Memory Caching</c:v>
+                  <c:v>CUDA Shared Memory Caching</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3903,7 +4101,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CUDA Time Vectorized</c:v>
+                  <c:v>CUDA Vectorization</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4037,6 +4235,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Square Array Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
@@ -4101,6 +4354,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
@@ -4757,6 +5065,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Array Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4819,6 +5182,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Relative Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6719,6 +7137,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CUDA Global Memory Coalescing</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7053,7 +7496,35 @@
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="5000"/>
+                    <a:lumOff val="95000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="74000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="45000"/>
+                    <a:lumOff val="55000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="83000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="45000"/>
+                    <a:lumOff val="55000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="30000"/>
+                    <a:lumOff val="70000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+            </a:gradFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -7148,6 +7619,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CUDA Vectorized</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7482,7 +7978,35 @@
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="5000"/>
+                    <a:lumOff val="95000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="74000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="45000"/>
+                    <a:lumOff val="55000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="83000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="45000"/>
+                    <a:lumOff val="55000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="30000"/>
+                    <a:lumOff val="70000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+            </a:gradFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -7577,6 +8101,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CUDA naive</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7911,7 +8460,35 @@
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="5000"/>
+                    <a:lumOff val="95000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="74000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="45000"/>
+                    <a:lumOff val="55000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="83000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="45000"/>
+                    <a:lumOff val="55000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="30000"/>
+                    <a:lumOff val="70000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+            </a:gradFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -15648,8 +16225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC22C78A-4AFB-42A7-860C-985947D40450}">
   <dimension ref="A1:AB64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q58" workbookViewId="0">
-      <selection activeCell="AC79" sqref="AC79"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15657,7 +16234,7 @@
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
@@ -15682,25 +16259,25 @@
         <v>31</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1</v>
+        <v>415</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>2</v>
+        <v>416</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>3</v>
+        <v>414</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>4</v>
+        <v>417</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>5</v>
+        <v>407</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>6</v>
+        <v>408</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>7</v>
+        <v>418</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Added a matlab figure generator and script to run it quickly. Updated comments and excel.
</commit_message>
<xml_diff>
--- a/Summarized Trials.xlsx
+++ b/Summarized Trials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e54ee0e16b764741/University/Fa2023/ECE 718 - Compiler Design for High Performance/Project/GemmCUDA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="610" documentId="13_ncr:1_{3C733FE7-E8A4-42C6-AC06-D019A0768725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{319C647E-9792-4F19-A458-80425D19BCB8}"/>
+  <xr:revisionPtr revIDLastSave="682" documentId="13_ncr:1_{3C733FE7-E8A4-42C6-AC06-D019A0768725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{626E2DAE-62E7-4477-B5A4-EFBA8DCC24AE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Trials" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,40 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Alex Barsan</author>
+  </authors>
+  <commentList>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{397A070B-EDF4-4CD4-BD33-A1753F505134}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Alex Barsan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+note 4096 is estimated… group policy restart after ~22 hours so it's already pretty egregious. </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Alex Barsan</author>
@@ -73,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="437">
   <si>
     <t>Trial Name</t>
   </si>
@@ -1375,14 +1409,24 @@
   </si>
   <si>
     <t>Trial 36</t>
+  </si>
+  <si>
+    <t>Trial 37</t>
+  </si>
+  <si>
+    <t>Trial 38</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1800,7 +1844,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1818,7 +1862,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1931,16 +1974,20 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2128,7 +2175,7 @@
             <c:numRef>
               <c:f>'Context and Graphs'!$B$2:$B$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.18351006507873541</c:v>
@@ -2233,7 +2280,7 @@
             <c:numRef>
               <c:f>'Context and Graphs'!$C$2:$C$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.3670196533203125</c:v>
@@ -2338,7 +2385,7 @@
             <c:numRef>
               <c:f>'Context and Graphs'!$D$2:$D$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.13962650299072271</c:v>
@@ -2443,7 +2490,7 @@
             <c:numRef>
               <c:f>'Context and Graphs'!$E$2:$E$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.27828621864318848</c:v>
@@ -2704,7 +2751,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3915,7 +3962,7 @@
             <c:numRef>
               <c:f>'Context and Graphs'!$M$2:$M$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>2.9919147491455078E-3</c:v>
@@ -4017,7 +4064,7 @@
             <c:numRef>
               <c:f>'Context and Graphs'!$N$2:$N$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.15810346603393549</c:v>
@@ -4226,6 +4273,7 @@
       <c:valAx>
         <c:axId val="964389984"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4244,7 +4292,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4488,42 +4536,42 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$A$5:$A$8</c:f>
+              <c:f>'Context and Graphs'!$A$7:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>256</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>512</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1024</c:v>
+                  <c:v>8192</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4096</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$M$5:$M$8</c:f>
+              <c:f>'Context and Graphs'!$M$7:$M$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.9862861633300781E-3</c:v>
+                  <c:v>8.6768388748168945E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.39617919921875E-2</c:v>
+                  <c:v>4.482025146484375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.6768388748168945E-2</c:v>
+                  <c:v>36.324334621429443</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.482025146484375</c:v>
+                  <c:v>289.1930079460144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4575,42 +4623,42 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$A$5:$A$8</c:f>
+              <c:f>'Context and Graphs'!$A$7:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>256</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>512</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1024</c:v>
+                  <c:v>8192</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4096</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$N$5:$N$8</c:f>
+              <c:f>'Context and Graphs'!$N$7:$N$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.17852139472961431</c:v>
+                  <c:v>0.19248294830322271</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18350934982299799</c:v>
+                  <c:v>0.80584812164306641</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19248294830322271</c:v>
+                  <c:v>3.0099761486053471</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.80584812164306641</c:v>
+                  <c:v>14.67776441574097</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4662,42 +4710,42 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$A$5:$A$8</c:f>
+              <c:f>'Context and Graphs'!$A$7:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>256</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>512</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1024</c:v>
+                  <c:v>8192</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4096</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$H$5:$H$8</c:f>
+              <c:f>'Context and Graphs'!$H$7:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.595759391784668E-2</c:v>
+                  <c:v>0.20322537422180181</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9868106842041023E-2</c:v>
+                  <c:v>10.46019577980042</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20322537422180181</c:v>
+                  <c:v>81.366543531417847</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.46019577980042</c:v>
+                  <c:v>664.83272767066956</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4724,6 +4772,8 @@
         <c:axId val="933281600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="16834"/>
+          <c:min val="1024"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4781,11 +4831,13 @@
         <c:crossAx val="964389984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="256"/>
+        <c:majorUnit val="1024"/>
+        <c:minorUnit val="128"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="964389984"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4804,7 +4856,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4844,7 +4896,8 @@
         <c:crossAx val="933281600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
+        <c:majorUnit val="10"/>
+        <c:minorUnit val="10"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -5048,10 +5101,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$A$2:$A$19</c:f>
+              <c:f>'Context and Graphs'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>32</c:v>
                 </c:pt>
@@ -5078,10 +5131,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$E$2:$E$19</c:f>
+              <c:f>'Context and Graphs'!$E$2:$E$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.27828621864318848</c:v>
                 </c:pt>
@@ -5153,10 +5206,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$A$2:$A$19</c:f>
+              <c:f>'Context and Graphs'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>32</c:v>
                 </c:pt>
@@ -5183,10 +5236,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$F$2:$F$19</c:f>
+              <c:f>'Context and Graphs'!$F$2:$F$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.1037919521331787</c:v>
                 </c:pt>
@@ -5258,10 +5311,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$A$2:$A$19</c:f>
+              <c:f>'Context and Graphs'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>32</c:v>
                 </c:pt>
@@ -5288,10 +5341,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$G$2:$G$19</c:f>
+              <c:f>'Context and Graphs'!$G$2:$G$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.16854977607727051</c:v>
                 </c:pt>
@@ -5369,10 +5422,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$A$2:$A$19</c:f>
+              <c:f>'Context and Graphs'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>32</c:v>
                 </c:pt>
@@ -5399,10 +5452,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Context and Graphs'!$H$2:$H$19</c:f>
+              <c:f>'Context and Graphs'!$H$2:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>7.9782009124755859E-3</c:v>
                 </c:pt>
@@ -5640,7 +5693,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
@@ -16977,15 +17030,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2219325</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:colOff>2028825</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17013,15 +17066,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2247900</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>2143125</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2324100</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>2219325</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17050,16 +17103,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>133351</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>438151</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17994,11 +18047,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18203,12 +18256,12 @@
         <v>0.20322537422180181</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" s="8">
+        <v>79200</v>
       </c>
       <c r="C8">
         <v>4724.1884799003601</v>
@@ -18824,7 +18877,7 @@
         <v>0</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>7.9782009124755859E-3</v>
       </c>
       <c r="I31">
         <v>2.9919147491455078E-3</v>
@@ -18856,7 +18909,7 @@
         <v>0</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>6.9811344146728524E-3</v>
       </c>
       <c r="I32">
         <v>2.990961074829102E-3</v>
@@ -18888,7 +18941,7 @@
         <v>0</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>7.9784393310546875E-3</v>
       </c>
       <c r="I33">
         <v>3.9889812469482422E-3</v>
@@ -18920,7 +18973,7 @@
         <v>0</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>1.595759391784668E-2</v>
       </c>
       <c r="I34">
         <v>4.9862861633300781E-3</v>
@@ -18952,7 +19005,7 @@
         <v>0</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>4.9868106842041023E-2</v>
       </c>
       <c r="I35">
         <v>1.39617919921875E-2</v>
@@ -18984,7 +19037,7 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>0.20322537422180181</v>
       </c>
       <c r="I36">
         <v>8.6768388748168945E-2</v>
@@ -19016,7 +19069,7 @@
         <v>0</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>10.25245118141174</v>
       </c>
       <c r="I37">
         <v>4.482025146484375</v>
@@ -19025,8 +19078,73 @@
         <v>0.80584812164306641</v>
       </c>
     </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>434</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>80.530763149261475</v>
+      </c>
+      <c r="F38">
+        <v>81.702349424362183</v>
+      </c>
+      <c r="G38">
+        <v>86.798654079437256</v>
+      </c>
+      <c r="H38">
+        <v>81.366543531417847</v>
+      </c>
+      <c r="I38">
+        <v>36.324334621429443</v>
+      </c>
+      <c r="J38">
+        <v>3.0099761486053471</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>435</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>663.6075005531311</v>
+      </c>
+      <c r="F39">
+        <v>666.01704597473145</v>
+      </c>
+      <c r="G39">
+        <v>683.79458785057068</v>
+      </c>
+      <c r="H39">
+        <v>664.83272767066956</v>
+      </c>
+      <c r="I39">
+        <v>289.1930079460144</v>
+      </c>
+      <c r="J39">
+        <v>14.67776441574097</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -19034,8 +19152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC22C78A-4AFB-42A7-860C-985947D40450}">
   <dimension ref="A1:AD64"/>
   <sheetViews>
-    <sheetView topLeftCell="H24" workbookViewId="0">
-      <selection activeCell="T66" sqref="T66"/>
+    <sheetView topLeftCell="S51" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19047,7 +19165,8 @@
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
@@ -19065,7 +19184,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -19083,7 +19202,7 @@
       <c r="F1" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>408</v>
       </c>
       <c r="H1" s="5" t="s">
@@ -19098,24 +19217,24 @@
       <c r="K1" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="18" t="s">
         <v>398</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="55" t="s">
         <v>419</v>
       </c>
-      <c r="N1" s="58" t="s">
+      <c r="N1" s="56" t="s">
         <v>420</v>
       </c>
-      <c r="Q1" s="65" t="s">
+      <c r="Q1" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="67"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="70"/>
       <c r="Z1" s="1" t="s">
         <v>4</v>
       </c>
@@ -19130,61 +19249,61 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
+      <c r="A2" s="10">
         <v>32</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="59">
         <v>0.18351006507873541</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="63">
         <v>0.3670196533203125</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="63">
         <v>0.13962650299072271</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="63">
         <v>0.27828621864318848</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="63">
         <v>0.1037919521331787</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="63">
         <v>0.16854977607727051</v>
       </c>
       <c r="H2" s="7">
         <v>7.9782009124755859E-3</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="12">
         <f>B2/E2</f>
         <v>0.65942922352912969</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="12">
         <f>B2/H2</f>
         <v>23.001434420105795</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="12">
         <f>B2/F2</f>
         <v>1.7680567838561116</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2" s="13">
         <f>B2/G2</f>
         <v>1.0887588779388615</v>
       </c>
-      <c r="M2" s="56">
+      <c r="M2" s="57">
         <v>2.9919147491455078E-3</v>
       </c>
-      <c r="N2" s="59">
+      <c r="N2" s="58">
         <v>0.15810346603393549</v>
       </c>
-      <c r="Q2" s="62" t="s">
+      <c r="Q2" s="65" t="s">
         <v>411</v>
       </c>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
-      <c r="W2" s="64"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="67"/>
       <c r="Y2" t="s">
         <v>15</v>
       </c>
@@ -19202,74 +19321,74 @@
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>64</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="59">
         <v>1.27190637588501</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="63">
         <v>0.36806845664978027</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="63">
         <v>0.1385462284088135</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="63">
         <v>0.27078390121459961</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="63">
         <v>9.7769021987915039E-2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="63">
         <v>0.16512465476989749</v>
       </c>
       <c r="H3" s="7">
         <v>6.9811344146728524E-3</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <f t="shared" ref="I3:I8" si="0">B3/E3</f>
         <v>4.6971270085846362</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="12">
         <f t="shared" ref="J3:J8" si="1">B3/H3</f>
         <v>182.19193333561014</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="12">
         <f t="shared" ref="K3:K8" si="2">B3/F3</f>
         <v>13.009298344441113</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="13">
         <f t="shared" ref="L3:L8" si="3">B3/G3</f>
         <v>7.7027042246200095</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="59">
         <v>2.990961074829102E-3</v>
       </c>
       <c r="N3" s="60">
         <v>0.18051719665527341</v>
       </c>
-      <c r="P3" s="44" t="s">
+      <c r="P3" s="43" t="s">
         <v>406</v>
       </c>
-      <c r="Q3" s="45">
+      <c r="Q3" s="44">
         <v>32</v>
       </c>
-      <c r="R3" s="46">
+      <c r="R3" s="45">
         <v>64</v>
       </c>
-      <c r="S3" s="46">
+      <c r="S3" s="45">
         <v>128</v>
       </c>
-      <c r="T3" s="46">
+      <c r="T3" s="45">
         <v>256</v>
       </c>
-      <c r="U3" s="46">
+      <c r="U3" s="45">
         <v>512</v>
       </c>
-      <c r="V3" s="46">
+      <c r="V3" s="45">
         <v>1024</v>
       </c>
-      <c r="W3" s="47">
+      <c r="W3" s="46">
         <v>4096</v>
       </c>
       <c r="Y3" t="s">
@@ -19289,74 +19408,74 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>128</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="59">
         <v>10.34896802902222</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="63">
         <v>0.39191865921020508</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="63">
         <v>0.16159248352050781</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="63">
         <v>0.28726029396057129</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="63">
         <v>9.9733114242553711E-2</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="63">
         <v>0.16655516624450681</v>
       </c>
       <c r="H4" s="7">
         <v>7.9784393310546875E-3</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="12">
         <f t="shared" si="0"/>
         <v>36.026447951914641</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="12">
         <f t="shared" si="1"/>
         <v>1297.116841979441</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="12">
         <f t="shared" si="2"/>
         <v>103.7666186162927</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="13">
         <f t="shared" si="3"/>
         <v>62.135376898664902</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="59">
         <v>3.9889812469482422E-3</v>
       </c>
       <c r="N4" s="60">
         <v>0.16954708099365229</v>
       </c>
-      <c r="P4" s="43" t="s">
+      <c r="P4" s="42" t="s">
         <v>405</v>
       </c>
-      <c r="Q4" s="48">
+      <c r="Q4" s="47">
         <v>0.65942922352912969</v>
       </c>
-      <c r="R4" s="49">
+      <c r="R4" s="48">
         <v>4.6971270085846362</v>
       </c>
-      <c r="S4" s="49">
+      <c r="S4" s="48">
         <v>36.026447951914641</v>
       </c>
-      <c r="T4" s="49">
+      <c r="T4" s="48">
         <v>292.18407069256534</v>
       </c>
-      <c r="U4" s="49">
+      <c r="U4" s="48">
         <v>2020.5602365341686</v>
       </c>
-      <c r="V4" s="49">
+      <c r="V4" s="48">
         <v>4913.6869072018962</v>
       </c>
-      <c r="W4" s="14">
+      <c r="W4" s="13">
         <v>7059.5759713484658</v>
       </c>
       <c r="Y4" t="s">
@@ -19376,47 +19495,47 @@
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>256</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="59">
         <v>81.884746313095093</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="63">
         <v>0.5326075553894043</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="63">
         <v>0.15954279899597171</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="63">
         <v>0.28025054931640619</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="63">
         <v>0.1057174205780029</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="63">
         <v>0.18051719665527341</v>
       </c>
       <c r="H5" s="7">
         <v>1.595759391784668E-2</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <f t="shared" si="0"/>
         <v>292.18407069256534</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="12">
         <f t="shared" si="1"/>
         <v>5131.3967967010803</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="12">
         <f t="shared" si="2"/>
         <v>774.56246913134783</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="13">
         <f t="shared" si="3"/>
         <v>453.61188756696225</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="59">
         <v>4.9862861633300781E-3</v>
       </c>
       <c r="N5" s="60">
@@ -19425,25 +19544,25 @@
       <c r="P5" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="Q5" s="50">
+      <c r="Q5" s="49">
         <v>1.7680567838561116</v>
       </c>
-      <c r="R5" s="51">
+      <c r="R5" s="50">
         <v>13.009298344441113</v>
       </c>
-      <c r="S5" s="51">
+      <c r="S5" s="50">
         <v>103.7666186162927</v>
       </c>
-      <c r="T5" s="51">
+      <c r="T5" s="50">
         <v>774.56246913134783</v>
       </c>
-      <c r="U5" s="51">
+      <c r="U5" s="50">
         <v>4552.8687922157378</v>
       </c>
-      <c r="V5" s="51">
+      <c r="V5" s="50">
         <v>17401.275495098595</v>
       </c>
-      <c r="W5" s="14">
+      <c r="W5" s="13">
         <v>7536.2075467550321</v>
       </c>
       <c r="Y5" t="s">
@@ -19463,47 +19582,47 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>512</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="59">
         <v>658.41065311431885</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="63">
         <v>2.4474935531616211</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="63">
         <v>0.35804367065429688</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="63">
         <v>0.32585549354553223</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="63">
         <v>0.14461445808410639</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="63">
         <v>0.21143388748168951</v>
       </c>
       <c r="H6" s="7">
         <v>4.9868106842041023E-2</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="12">
         <f t="shared" si="0"/>
         <v>2020.5602365341686</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="12">
         <f t="shared" si="1"/>
         <v>13203.040877406029</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="12">
         <f t="shared" si="2"/>
         <v>4552.8687922157378</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="13">
         <f t="shared" si="3"/>
         <v>3114.0261429064353</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="59">
         <v>1.39617919921875E-2</v>
       </c>
       <c r="N6" s="60">
@@ -19512,25 +19631,25 @@
       <c r="P6" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="Q6" s="50">
+      <c r="Q6" s="49">
         <v>1.0887588779388615</v>
       </c>
-      <c r="R6" s="51">
+      <c r="R6" s="50">
         <v>7.7027042246200095</v>
       </c>
-      <c r="S6" s="51">
+      <c r="S6" s="50">
         <v>62.135376898664902</v>
       </c>
-      <c r="T6" s="51">
+      <c r="T6" s="50">
         <v>453.61188756696225</v>
       </c>
-      <c r="U6" s="51">
+      <c r="U6" s="50">
         <v>3114.0261429064353</v>
       </c>
-      <c r="V6" s="51">
+      <c r="V6" s="50">
         <v>14070.88570815296</v>
       </c>
-      <c r="W6" s="52">
+      <c r="W6" s="51">
         <v>6981.7071005182797</v>
       </c>
       <c r="Y6" t="s">
@@ -19550,74 +19669,74 @@
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>1024</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="59">
         <v>5501.495353937149</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="63">
         <v>16.37320613861084</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="63">
         <v>1.764312267303467</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="63">
         <v>1.1196267604827881</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="63">
         <v>0.31615471839904791</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="63">
         <v>0.39098429679870611</v>
       </c>
       <c r="H7" s="7">
         <v>0.20322537422180181</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="12">
         <f t="shared" si="0"/>
         <v>4913.6869072018962</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="12">
         <f t="shared" si="1"/>
         <v>27070.907729921426</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="12">
         <f t="shared" si="2"/>
         <v>17401.275495098595</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="13">
         <f t="shared" si="3"/>
         <v>14070.88570815296</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="59">
         <v>8.6768388748168945E-2</v>
       </c>
       <c r="N7" s="60">
         <v>0.19248294830322271</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="P7" s="14" t="s">
         <v>409</v>
       </c>
-      <c r="Q7" s="53">
+      <c r="Q7" s="52">
         <v>23.001434420105795</v>
       </c>
-      <c r="R7" s="54">
+      <c r="R7" s="53">
         <v>182.19193333561</v>
       </c>
-      <c r="S7" s="54">
+      <c r="S7" s="53">
         <v>1297.116841979441</v>
       </c>
-      <c r="T7" s="54">
+      <c r="T7" s="53">
         <v>5131.3967967010803</v>
       </c>
-      <c r="U7" s="54">
+      <c r="U7" s="53">
         <v>13203.040877406029</v>
       </c>
-      <c r="V7" s="54">
+      <c r="V7" s="53">
         <v>27070.907729921426</v>
       </c>
-      <c r="W7" s="55">
+      <c r="W7" s="54">
         <v>7571.5600039668789</v>
       </c>
       <c r="Y7" t="s">
@@ -19637,50 +19756,50 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
+      <c r="A8" s="11">
         <v>4096</v>
       </c>
       <c r="B8" s="8">
         <v>79200</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="64">
         <v>4724.1884799003601</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="64">
         <v>163.39830279350281</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="64">
         <v>11.21880412101746</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="64">
         <v>10.509264707565309</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="64">
         <v>11.34393048286438</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <v>10.46019577980042</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="15">
         <f t="shared" si="0"/>
         <v>7059.5759713484658</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="15">
         <f t="shared" si="1"/>
         <v>7571.5600039668789</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="15">
         <f t="shared" si="2"/>
         <v>7536.2075467550321</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="16">
         <f t="shared" si="3"/>
         <v>6981.7071005182797</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="61">
         <v>4.482025146484375</v>
       </c>
-      <c r="N8" s="61">
+      <c r="N8" s="62">
         <v>0.80584812164306641</v>
       </c>
       <c r="Y8" t="s">
@@ -19700,24 +19819,83 @@
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="Y9" s="20" t="s">
+      <c r="A9" s="10">
+        <v>8192</v>
+      </c>
+      <c r="B9" t="s">
+        <v>436</v>
+      </c>
+      <c r="C9" t="s">
+        <v>436</v>
+      </c>
+      <c r="D9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E9" s="63">
+        <v>80.530763149261475</v>
+      </c>
+      <c r="F9" s="63">
+        <v>81.702349424362183</v>
+      </c>
+      <c r="G9" s="63">
+        <v>86.798654079437256</v>
+      </c>
+      <c r="H9">
+        <v>81.366543531417847</v>
+      </c>
+      <c r="M9" s="63">
+        <v>36.324334621429443</v>
+      </c>
+      <c r="N9" s="63">
+        <v>3.0099761486053471</v>
+      </c>
+      <c r="Y9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="20">
+      <c r="Z9" s="19">
         <v>7.8307175636291504</v>
       </c>
-      <c r="AA9" s="20">
+      <c r="AA9" s="19">
         <v>7.6611173152923584</v>
       </c>
-      <c r="AB9" s="20">
+      <c r="AB9" s="19">
         <v>41.8465895652771</v>
       </c>
-      <c r="AC9" s="20">
+      <c r="AC9" s="19">
         <v>7.6051571369171143</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="19">
+        <v>16384</v>
+      </c>
+      <c r="B10" t="s">
+        <v>436</v>
+      </c>
+      <c r="C10" t="s">
+        <v>436</v>
+      </c>
+      <c r="D10" t="s">
+        <v>436</v>
+      </c>
+      <c r="E10" s="63">
+        <v>663.6075005531311</v>
+      </c>
+      <c r="F10" s="63">
+        <v>666.01704597473145</v>
+      </c>
+      <c r="G10" s="63">
+        <v>683.79458785057068</v>
+      </c>
+      <c r="H10">
+        <v>664.83272767066956</v>
+      </c>
+      <c r="M10" s="63">
+        <v>289.1930079460144</v>
+      </c>
+      <c r="N10" s="63">
+        <v>14.67776441574097</v>
+      </c>
       <c r="Y10" t="s">
         <v>23</v>
       </c>
@@ -19882,30 +20060,30 @@
       <c r="B19" s="2"/>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Y21" s="22" t="s">
+      <c r="Y21" s="21" t="s">
         <v>413</v>
       </c>
-      <c r="Z21" s="22" t="s">
+      <c r="Z21" s="21" t="s">
         <v>412</v>
       </c>
-      <c r="AA21" s="42" t="s">
+      <c r="AA21" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="AB21" s="42" t="s">
+      <c r="AB21" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="AC21" s="42" t="s">
+      <c r="AC21" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="AD21" s="42" t="s">
+      <c r="AD21" s="41" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Y22" s="21">
+      <c r="Y22" s="20">
         <v>4</v>
       </c>
-      <c r="Z22" s="21">
+      <c r="Z22" s="20">
         <v>4</v>
       </c>
       <c r="AA22">
@@ -19922,10 +20100,10 @@
       </c>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Y23" s="21">
+      <c r="Y23" s="20">
         <v>4</v>
       </c>
-      <c r="Z23" s="21">
+      <c r="Z23" s="20">
         <v>8</v>
       </c>
       <c r="AA23">
@@ -19942,10 +20120,10 @@
       </c>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Y24" s="21">
+      <c r="Y24" s="20">
         <v>4</v>
       </c>
-      <c r="Z24" s="21">
+      <c r="Z24" s="20">
         <v>16</v>
       </c>
       <c r="AA24">
@@ -19962,10 +20140,10 @@
       </c>
     </row>
     <row r="25" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Y25" s="21">
+      <c r="Y25" s="20">
         <v>4</v>
       </c>
-      <c r="Z25" s="21">
+      <c r="Z25" s="20">
         <v>32</v>
       </c>
       <c r="AA25">
@@ -19982,10 +20160,10 @@
       </c>
     </row>
     <row r="26" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Y26" s="21">
+      <c r="Y26" s="20">
         <v>8</v>
       </c>
-      <c r="Z26" s="21">
+      <c r="Z26" s="20">
         <v>4</v>
       </c>
       <c r="AA26">
@@ -20002,10 +20180,10 @@
       </c>
     </row>
     <row r="27" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Y27" s="21">
+      <c r="Y27" s="20">
         <v>8</v>
       </c>
-      <c r="Z27" s="21">
+      <c r="Z27" s="20">
         <v>8</v>
       </c>
       <c r="AA27">
@@ -20022,10 +20200,10 @@
       </c>
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Y28" s="21">
+      <c r="Y28" s="20">
         <v>8</v>
       </c>
-      <c r="Z28" s="21">
+      <c r="Z28" s="20">
         <v>16</v>
       </c>
       <c r="AA28">
@@ -20042,30 +20220,30 @@
       </c>
     </row>
     <row r="29" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Y29" s="21">
+      <c r="Y29" s="20">
         <v>8</v>
       </c>
-      <c r="Z29" s="21">
+      <c r="Z29" s="20">
         <v>32</v>
       </c>
-      <c r="AA29" s="20">
+      <c r="AA29" s="19">
         <v>7.8307175636291504</v>
       </c>
-      <c r="AB29" s="20">
+      <c r="AB29" s="19">
         <v>7.6611173152923584</v>
       </c>
-      <c r="AC29" s="20">
+      <c r="AC29" s="19">
         <v>41.8465895652771</v>
       </c>
-      <c r="AD29" s="20">
+      <c r="AD29" s="19">
         <v>7.6051571369171143</v>
       </c>
     </row>
     <row r="30" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Y30" s="21">
+      <c r="Y30" s="20">
         <v>16</v>
       </c>
-      <c r="Z30" s="21">
+      <c r="Z30" s="20">
         <v>4</v>
       </c>
       <c r="AA30">
@@ -20079,10 +20257,10 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Y31" s="21">
+      <c r="Y31" s="20">
         <v>16</v>
       </c>
-      <c r="Z31" s="21">
+      <c r="Z31" s="20">
         <v>8</v>
       </c>
       <c r="AA31">
@@ -20096,10 +20274,10 @@
       </c>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="Y32" s="21">
+      <c r="Y32" s="20">
         <v>16</v>
       </c>
-      <c r="Z32" s="21">
+      <c r="Z32" s="20">
         <v>16</v>
       </c>
       <c r="AA32">
@@ -20119,10 +20297,10 @@
       <c r="A33" t="s">
         <v>399</v>
       </c>
-      <c r="Y33" s="21">
+      <c r="Y33" s="20">
         <v>16</v>
       </c>
-      <c r="Z33" s="21">
+      <c r="Z33" s="20">
         <v>32</v>
       </c>
       <c r="AA33">
@@ -20138,35 +20316,35 @@
         <v>10.497905492782589</v>
       </c>
     </row>
-    <row r="34" spans="1:30" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="25" t="s">
+    <row r="34" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="C34" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="D34" s="25" t="s">
         <v>401</v>
       </c>
-      <c r="E34" s="26" t="s">
+      <c r="E34" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="26" t="s">
+      <c r="F34" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="26" t="s">
+      <c r="G34" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="H34" s="26" t="s">
+      <c r="H34" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="I34" s="27" t="s">
+      <c r="I34" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="Y34" s="21">
+      <c r="Y34" s="20">
         <v>32</v>
       </c>
-      <c r="Z34" s="21">
+      <c r="Z34" s="20">
         <v>4</v>
       </c>
       <c r="AA34">
@@ -20180,25 +20358,25 @@
         <v>20.98466849327087</v>
       </c>
     </row>
-    <row r="35" spans="1:30" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="28" t="s">
+    <row r="35" spans="1:30" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="24">
+      <c r="C35" s="22"/>
+      <c r="D35" s="23">
         <v>137.53242468833901</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="29" t="s">
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="28" t="s">
         <v>402</v>
       </c>
-      <c r="Y35" s="21">
+      <c r="Y35" s="20">
         <v>32</v>
       </c>
-      <c r="Z35" s="21">
+      <c r="Z35" s="20">
         <v>8</v>
       </c>
       <c r="AA35">
@@ -20213,34 +20391,34 @@
       </c>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="C36" s="31">
+      <c r="C36" s="30">
         <v>0.99490000000000001</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="20">
         <v>10</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="F36" s="20" t="s">
         <v>342</v>
       </c>
-      <c r="G36" s="21" t="s">
+      <c r="G36" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="H36" s="21" t="s">
+      <c r="H36" s="20" t="s">
         <v>344</v>
       </c>
-      <c r="I36" s="32" t="s">
+      <c r="I36" s="31" t="s">
         <v>400</v>
       </c>
-      <c r="Y36" s="21">
+      <c r="Y36" s="20">
         <v>32</v>
       </c>
-      <c r="Z36" s="21">
+      <c r="Z36" s="20">
         <v>16</v>
       </c>
       <c r="AA36">
@@ -20254,32 +20432,32 @@
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B37" s="30"/>
-      <c r="C37" s="31">
+      <c r="B37" s="29"/>
+      <c r="C37" s="30">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D37" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="E37" s="21">
+      <c r="E37" s="20">
         <v>20</v>
       </c>
-      <c r="F37" s="21" t="s">
+      <c r="F37" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="G37" s="21" t="s">
+      <c r="G37" s="20" t="s">
         <v>347</v>
       </c>
-      <c r="H37" s="21" t="s">
+      <c r="H37" s="20" t="s">
         <v>348</v>
       </c>
-      <c r="I37" s="33" t="s">
+      <c r="I37" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="Y37" s="21">
+      <c r="Y37" s="20">
         <v>32</v>
       </c>
-      <c r="Z37" s="21">
+      <c r="Z37" s="20">
         <v>32</v>
       </c>
       <c r="AA37">
@@ -20296,644 +20474,644 @@
       </c>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B38" s="30"/>
-      <c r="C38" s="31">
+      <c r="B38" s="29"/>
+      <c r="C38" s="30">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="20" t="s">
         <v>349</v>
       </c>
-      <c r="E38" s="21">
+      <c r="E38" s="20">
         <v>10</v>
       </c>
-      <c r="F38" s="21" t="s">
+      <c r="F38" s="20" t="s">
         <v>350</v>
       </c>
-      <c r="G38" s="21" t="s">
+      <c r="G38" s="20" t="s">
         <v>351</v>
       </c>
-      <c r="H38" s="21" t="s">
+      <c r="H38" s="20" t="s">
         <v>352</v>
       </c>
-      <c r="I38" s="33" t="s">
+      <c r="I38" s="32" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="C39" s="31">
+      <c r="C39" s="30">
         <v>0.99729999999999996</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="20" t="s">
         <v>353</v>
       </c>
-      <c r="E39" s="21">
+      <c r="E39" s="20">
         <v>10</v>
       </c>
-      <c r="F39" s="21" t="s">
+      <c r="F39" s="20" t="s">
         <v>354</v>
       </c>
-      <c r="G39" s="21" t="s">
+      <c r="G39" s="20" t="s">
         <v>355</v>
       </c>
-      <c r="H39" s="21" t="s">
+      <c r="H39" s="20" t="s">
         <v>356</v>
       </c>
-      <c r="I39" s="33" t="s">
+      <c r="I39" s="32" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B40" s="30"/>
-      <c r="C40" s="31">
+      <c r="B40" s="29"/>
+      <c r="C40" s="30">
         <v>1.8E-3</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="D40" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="E40" s="21">
+      <c r="E40" s="20">
         <v>20</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F40" s="20" t="s">
         <v>358</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="G40" s="20" t="s">
         <v>359</v>
       </c>
-      <c r="H40" s="21" t="s">
+      <c r="H40" s="20" t="s">
         <v>360</v>
       </c>
-      <c r="I40" s="33" t="s">
+      <c r="I40" s="32" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B41" s="30"/>
-      <c r="C41" s="31">
+      <c r="B41" s="29"/>
+      <c r="C41" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="D41" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="E41" s="21">
+      <c r="E41" s="20">
         <v>1</v>
       </c>
-      <c r="F41" s="21" t="s">
+      <c r="F41" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="G41" s="21" t="s">
+      <c r="G41" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="H41" s="21" t="s">
+      <c r="H41" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="I41" s="33" t="s">
+      <c r="I41" s="32" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B42" s="30"/>
-      <c r="C42" s="31">
+      <c r="B42" s="29"/>
+      <c r="C42" s="30">
         <v>1E-4</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D42" s="20" t="s">
         <v>362</v>
       </c>
-      <c r="E42" s="21">
+      <c r="E42" s="20">
         <v>1</v>
       </c>
-      <c r="F42" s="21" t="s">
+      <c r="F42" s="20" t="s">
         <v>362</v>
       </c>
-      <c r="G42" s="21" t="s">
+      <c r="G42" s="20" t="s">
         <v>362</v>
       </c>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="20" t="s">
         <v>362</v>
       </c>
-      <c r="I42" s="33" t="s">
+      <c r="I42" s="32" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B43" s="30"/>
-      <c r="C43" s="31">
+      <c r="B43" s="29"/>
+      <c r="C43" s="30">
         <v>1E-4</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="D43" s="20" t="s">
         <v>363</v>
       </c>
-      <c r="E43" s="21">
+      <c r="E43" s="20">
         <v>22</v>
       </c>
-      <c r="F43" s="21" t="s">
+      <c r="F43" s="20" t="s">
         <v>364</v>
       </c>
-      <c r="G43" s="21" t="s">
+      <c r="G43" s="20" t="s">
         <v>365</v>
       </c>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="20" t="s">
         <v>366</v>
       </c>
-      <c r="I43" s="33" t="s">
+      <c r="I43" s="32" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="34"/>
-      <c r="C44" s="35">
+      <c r="B44" s="33"/>
+      <c r="C44" s="34">
         <v>1E-4</v>
       </c>
-      <c r="D44" s="36" t="s">
+      <c r="D44" s="35" t="s">
         <v>367</v>
       </c>
-      <c r="E44" s="36">
+      <c r="E44" s="35">
         <v>30</v>
       </c>
-      <c r="F44" s="36" t="s">
+      <c r="F44" s="35" t="s">
         <v>368</v>
       </c>
-      <c r="G44" s="36" t="s">
+      <c r="G44" s="35" t="s">
         <v>369</v>
       </c>
-      <c r="H44" s="36" t="s">
+      <c r="H44" s="35" t="s">
         <v>370</v>
       </c>
-      <c r="I44" s="37" t="s">
+      <c r="I44" s="36" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="39"/>
-      <c r="D45" s="40">
+      <c r="C45" s="38"/>
+      <c r="D45" s="39">
         <v>4.7253768444061297</v>
       </c>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="41" t="s">
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="40" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="C46" s="31">
+      <c r="C46" s="30">
         <v>0.85189999999999999</v>
       </c>
-      <c r="D46" s="21" t="s">
+      <c r="D46" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="E46" s="21">
+      <c r="E46" s="20">
         <v>10</v>
       </c>
-      <c r="F46" s="21" t="s">
+      <c r="F46" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="G46" s="21" t="s">
+      <c r="G46" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="I46" s="32" t="s">
+      <c r="I46" s="31" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B47" s="30"/>
-      <c r="C47" s="31">
+      <c r="B47" s="29"/>
+      <c r="C47" s="30">
         <v>0.11609999999999999</v>
       </c>
-      <c r="D47" s="21" t="s">
+      <c r="D47" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="E47" s="21">
+      <c r="E47" s="20">
         <v>20</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="F47" s="20" t="s">
         <v>294</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="G47" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="H47" s="21" t="s">
+      <c r="H47" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="I47" s="33" t="s">
+      <c r="I47" s="32" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B48" s="30"/>
-      <c r="C48" s="31">
+      <c r="B48" s="29"/>
+      <c r="C48" s="30">
         <v>3.1899999999999998E-2</v>
       </c>
-      <c r="D48" s="21" t="s">
+      <c r="D48" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="E48" s="21">
+      <c r="E48" s="20">
         <v>10</v>
       </c>
-      <c r="F48" s="21" t="s">
+      <c r="F48" s="20" t="s">
         <v>298</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="G48" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="H48" s="21" t="s">
+      <c r="H48" s="20" t="s">
         <v>300</v>
       </c>
-      <c r="I48" s="33" t="s">
+      <c r="I48" s="32" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="C49" s="31">
+      <c r="C49" s="30">
         <v>0.91690000000000005</v>
       </c>
-      <c r="D49" s="21" t="s">
+      <c r="D49" s="20" t="s">
         <v>301</v>
       </c>
-      <c r="E49" s="21">
+      <c r="E49" s="20">
         <v>10</v>
       </c>
-      <c r="F49" s="21" t="s">
+      <c r="F49" s="20" t="s">
         <v>302</v>
       </c>
-      <c r="G49" s="21" t="s">
+      <c r="G49" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="H49" s="21" t="s">
+      <c r="H49" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="I49" s="33" t="s">
+      <c r="I49" s="32" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="30"/>
-      <c r="C50" s="31">
+      <c r="B50" s="29"/>
+      <c r="C50" s="30">
         <v>5.3699999999999998E-2</v>
       </c>
-      <c r="D50" s="21" t="s">
+      <c r="D50" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="E50" s="21">
+      <c r="E50" s="20">
         <v>20</v>
       </c>
-      <c r="F50" s="21" t="s">
+      <c r="F50" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="G50" s="21" t="s">
+      <c r="G50" s="20" t="s">
         <v>307</v>
       </c>
-      <c r="H50" s="21" t="s">
+      <c r="H50" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="I50" s="33" t="s">
+      <c r="I50" s="32" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="30"/>
-      <c r="C51" s="31">
+      <c r="B51" s="29"/>
+      <c r="C51" s="30">
         <v>0.02</v>
       </c>
-      <c r="D51" s="21" t="s">
+      <c r="D51" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="E51" s="21">
+      <c r="E51" s="20">
         <v>1</v>
       </c>
-      <c r="F51" s="21" t="s">
+      <c r="F51" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="G51" s="21" t="s">
+      <c r="G51" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="H51" s="21" t="s">
+      <c r="H51" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="I51" s="33" t="s">
+      <c r="I51" s="32" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="30"/>
-      <c r="C52" s="31">
+      <c r="B52" s="29"/>
+      <c r="C52" s="30">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D52" s="21" t="s">
+      <c r="D52" s="20" t="s">
         <v>310</v>
       </c>
-      <c r="E52" s="21">
+      <c r="E52" s="20">
         <v>1</v>
       </c>
-      <c r="F52" s="21" t="s">
+      <c r="F52" s="20" t="s">
         <v>310</v>
       </c>
-      <c r="G52" s="21" t="s">
+      <c r="G52" s="20" t="s">
         <v>310</v>
       </c>
-      <c r="H52" s="21" t="s">
+      <c r="H52" s="20" t="s">
         <v>310</v>
       </c>
-      <c r="I52" s="33" t="s">
+      <c r="I52" s="32" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="30"/>
-      <c r="C53" s="31">
+      <c r="B53" s="29"/>
+      <c r="C53" s="30">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="D53" s="21" t="s">
+      <c r="D53" s="20" t="s">
         <v>311</v>
       </c>
-      <c r="E53" s="21">
+      <c r="E53" s="20">
         <v>22</v>
       </c>
-      <c r="F53" s="21" t="s">
+      <c r="F53" s="20" t="s">
         <v>312</v>
       </c>
-      <c r="G53" s="21" t="s">
+      <c r="G53" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="H53" s="21" t="s">
+      <c r="H53" s="20" t="s">
         <v>314</v>
       </c>
-      <c r="I53" s="33" t="s">
+      <c r="I53" s="32" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="54" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="34"/>
-      <c r="C54" s="35">
+      <c r="B54" s="33"/>
+      <c r="C54" s="34">
         <v>1.5E-3</v>
       </c>
-      <c r="D54" s="36" t="s">
+      <c r="D54" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="E54" s="36">
+      <c r="E54" s="35">
         <v>30</v>
       </c>
-      <c r="F54" s="36" t="s">
+      <c r="F54" s="35" t="s">
         <v>316</v>
       </c>
-      <c r="G54" s="36" t="s">
+      <c r="G54" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="H54" s="36" t="s">
+      <c r="H54" s="35" t="s">
         <v>318</v>
       </c>
-      <c r="I54" s="37" t="s">
+      <c r="I54" s="36" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="55" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="38" t="s">
+      <c r="B55" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C55" s="39"/>
-      <c r="D55" s="40">
+      <c r="C55" s="38"/>
+      <c r="D55" s="39">
         <v>41.8465895652771</v>
       </c>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="39"/>
-      <c r="I55" s="41" t="s">
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
+      <c r="I55" s="40" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="30" t="s">
+      <c r="B56" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="C56" s="31">
+      <c r="C56" s="30">
         <v>0.98340000000000005</v>
       </c>
-      <c r="D56" s="21" t="s">
+      <c r="D56" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="E56" s="21">
+      <c r="E56" s="20">
         <v>10</v>
       </c>
-      <c r="F56" s="21" t="s">
+      <c r="F56" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="G56" s="21" t="s">
+      <c r="G56" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="H56" s="21" t="s">
+      <c r="H56" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="I56" s="33" t="s">
+      <c r="I56" s="32" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="30"/>
-      <c r="C57" s="31">
+      <c r="B57" s="29"/>
+      <c r="C57" s="30">
         <v>1.29E-2</v>
       </c>
-      <c r="D57" s="21" t="s">
+      <c r="D57" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="E57" s="21">
+      <c r="E57" s="20">
         <v>20</v>
       </c>
-      <c r="F57" s="21" t="s">
+      <c r="F57" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="G57" s="21" t="s">
+      <c r="G57" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="H57" s="21" t="s">
+      <c r="H57" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="I57" s="33" t="s">
+      <c r="I57" s="32" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="30"/>
-      <c r="C58" s="31">
+      <c r="B58" s="29"/>
+      <c r="C58" s="30">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="D58" s="21" t="s">
+      <c r="D58" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="E58" s="21">
+      <c r="E58" s="20">
         <v>10</v>
       </c>
-      <c r="F58" s="21" t="s">
+      <c r="F58" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="G58" s="21" t="s">
+      <c r="G58" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="H58" s="21" t="s">
+      <c r="H58" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="I58" s="33" t="s">
+      <c r="I58" s="32" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="30" t="s">
+      <c r="B59" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="C59" s="31">
+      <c r="C59" s="30">
         <v>0.99150000000000005</v>
       </c>
-      <c r="D59" s="21" t="s">
+      <c r="D59" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="E59" s="21">
+      <c r="E59" s="20">
         <v>10</v>
       </c>
-      <c r="F59" s="21" t="s">
+      <c r="F59" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="G59" s="21" t="s">
+      <c r="G59" s="20" t="s">
         <v>252</v>
       </c>
-      <c r="H59" s="21" t="s">
+      <c r="H59" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="I59" s="33" t="s">
+      <c r="I59" s="32" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="30"/>
-      <c r="C60" s="31">
+      <c r="B60" s="29"/>
+      <c r="C60" s="30">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="D60" s="21" t="s">
+      <c r="D60" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="E60" s="21">
+      <c r="E60" s="20">
         <v>20</v>
       </c>
-      <c r="F60" s="21" t="s">
+      <c r="F60" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="G60" s="21" t="s">
+      <c r="G60" s="20" t="s">
         <v>256</v>
       </c>
-      <c r="H60" s="21" t="s">
+      <c r="H60" s="20" t="s">
         <v>257</v>
       </c>
-      <c r="I60" s="33" t="s">
+      <c r="I60" s="32" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="30"/>
-      <c r="C61" s="31">
+      <c r="B61" s="29"/>
+      <c r="C61" s="30">
         <v>1.9E-3</v>
       </c>
-      <c r="D61" s="21" t="s">
+      <c r="D61" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="E61" s="21">
+      <c r="E61" s="20">
         <v>1</v>
       </c>
-      <c r="F61" s="21" t="s">
+      <c r="F61" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="G61" s="21" t="s">
+      <c r="G61" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="H61" s="21" t="s">
+      <c r="H61" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="I61" s="33" t="s">
+      <c r="I61" s="32" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="30"/>
-      <c r="C62" s="31">
+      <c r="B62" s="29"/>
+      <c r="C62" s="30">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D62" s="21" t="s">
+      <c r="D62" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="E62" s="21">
+      <c r="E62" s="20">
         <v>1</v>
       </c>
-      <c r="F62" s="21" t="s">
+      <c r="F62" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="G62" s="21" t="s">
+      <c r="G62" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="H62" s="21" t="s">
+      <c r="H62" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="I62" s="33" t="s">
+      <c r="I62" s="32" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="30"/>
-      <c r="C63" s="31">
+      <c r="B63" s="29"/>
+      <c r="C63" s="30">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D63" s="21" t="s">
+      <c r="D63" s="20" t="s">
         <v>260</v>
       </c>
-      <c r="E63" s="21">
+      <c r="E63" s="20">
         <v>22</v>
       </c>
-      <c r="F63" s="21" t="s">
+      <c r="F63" s="20" t="s">
         <v>261</v>
       </c>
-      <c r="G63" s="21" t="s">
+      <c r="G63" s="20" t="s">
         <v>262</v>
       </c>
-      <c r="H63" s="21" t="s">
+      <c r="H63" s="20" t="s">
         <v>263</v>
       </c>
-      <c r="I63" s="33" t="s">
+      <c r="I63" s="32" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="64" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="34"/>
-      <c r="C64" s="35">
+      <c r="B64" s="33"/>
+      <c r="C64" s="34">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D64" s="36" t="s">
+      <c r="D64" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="E64" s="36">
+      <c r="E64" s="35">
         <v>30</v>
       </c>
-      <c r="F64" s="36" t="s">
+      <c r="F64" s="35" t="s">
         <v>265</v>
       </c>
-      <c r="G64" s="36" t="s">
+      <c r="G64" s="35" t="s">
         <v>266</v>
       </c>
-      <c r="H64" s="36" t="s">
+      <c r="H64" s="35" t="s">
         <v>267</v>
       </c>
-      <c r="I64" s="37" t="s">
+      <c r="I64" s="36" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated with GFLOPS calculations for C++ comparison
</commit_message>
<xml_diff>
--- a/Summarized Trials.xlsx
+++ b/Summarized Trials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e54ee0e16b764741/University/Fa2023/ECE 718 - Compiler Design for High Performance/Project/GemmCUDA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="682" documentId="13_ncr:1_{3C733FE7-E8A4-42C6-AC06-D019A0768725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{626E2DAE-62E7-4477-B5A4-EFBA8DCC24AE}"/>
+  <xr:revisionPtr revIDLastSave="696" documentId="13_ncr:1_{3C733FE7-E8A4-42C6-AC06-D019A0768725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C57D4296-893C-4E1D-9528-2A696B57576C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Trials" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="448">
   <si>
     <t>Trial Name</t>
   </si>
@@ -1418,6 +1418,39 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>JIT</t>
+  </si>
+  <si>
+    <t>Loop Reordered JIT</t>
+  </si>
+  <si>
+    <t>Basic CUDA Kernel</t>
+  </si>
+  <si>
+    <t>General Memory Coalescing</t>
+  </si>
+  <si>
+    <t>Shared Memory Caching</t>
+  </si>
+  <si>
+    <t>Vectorized Kernel</t>
+  </si>
+  <si>
+    <t>MKL</t>
+  </si>
+  <si>
+    <t>cuBLAS</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>GFLOPS/s</t>
   </si>
 </sst>
 </file>
@@ -1844,7 +1877,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2004,6 +2037,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -18050,8 +18086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18270,7 +18306,7 @@
         <v>163.39830279350281</v>
       </c>
       <c r="E8">
-        <v>11.21880412101746</v>
+        <v>11.2188041210175</v>
       </c>
       <c r="F8">
         <v>10.509264707565309</v>
@@ -18452,7 +18488,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>7.7481474876403809</v>
+        <v>7.74814748764038</v>
       </c>
       <c r="F15">
         <v>7.6283092498779297</v>
@@ -19150,10 +19186,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC22C78A-4AFB-42A7-860C-985947D40450}">
-  <dimension ref="A1:AD64"/>
+  <dimension ref="A1:AG64"/>
   <sheetViews>
-    <sheetView topLeftCell="S51" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AG12" sqref="AG12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19181,9 +19217,11 @@
     <col min="27" max="28" width="36" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>31</v>
       </c>
@@ -19247,8 +19285,14 @@
       <c r="AC1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AF1" s="71" t="s">
+        <v>446</v>
+      </c>
+      <c r="AG1" s="71" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>32</v>
       </c>
@@ -19319,8 +19363,14 @@
       <c r="AC2">
         <v>13.90225052833557</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AF2" t="s">
+        <v>437</v>
+      </c>
+      <c r="AG2">
+        <v>1.7353403216161601E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>64</v>
       </c>
@@ -19406,8 +19456,14 @@
       <c r="AC3">
         <v>13.905861854553221</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AF3" t="s">
+        <v>438</v>
+      </c>
+      <c r="AG3">
+        <v>2.90926058637903E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>128</v>
       </c>
@@ -19493,8 +19549,14 @@
       <c r="AC4">
         <v>13.895543098449711</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AF4" t="s">
+        <v>439</v>
+      </c>
+      <c r="AG4">
+        <v>0.84112840294118996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>256</v>
       </c>
@@ -19580,8 +19642,14 @@
       <c r="AC5">
         <v>13.904776096343991</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AF5" t="s">
+        <v>440</v>
+      </c>
+      <c r="AG5">
+        <v>17.738298566365501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>512</v>
       </c>
@@ -19667,8 +19735,14 @@
       <c r="AC6">
         <v>7.5108833312988281</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AF6" t="s">
+        <v>441</v>
+      </c>
+      <c r="AG6">
+        <v>18.0753100449196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>1024</v>
       </c>
@@ -19754,8 +19828,14 @@
       <c r="AC7">
         <v>7.5578842163085938</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AF7" t="s">
+        <v>442</v>
+      </c>
+      <c r="AG7">
+        <v>29.0852894906571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>4096</v>
       </c>
@@ -19817,8 +19897,14 @@
       <c r="AC8">
         <v>7.5695807933807373</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AF8" t="s">
+        <v>443</v>
+      </c>
+      <c r="AG8">
+        <v>18.298640440768601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8192</v>
       </c>
@@ -19864,8 +19950,14 @@
       <c r="AC9" s="19">
         <v>7.6051571369171143</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AF9" t="s">
+        <v>444</v>
+      </c>
+      <c r="AG9">
+        <v>30.6644762088862</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>16384</v>
       </c>
@@ -19911,8 +20003,14 @@
       <c r="AC10">
         <v>10.54792332649231</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AF10" t="s">
+        <v>445</v>
+      </c>
+      <c r="AG10">
+        <v>170.55193128920101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="Y11" t="s">
         <v>24</v>
       </c>
@@ -19929,7 +20027,7 @@
         <v>10.497905492782589</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="Y12" t="s">
         <v>25</v>
       </c>
@@ -19946,7 +20044,7 @@
         <v>21.146031141281131</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -19966,7 +20064,7 @@
         <v>10.286246299743651</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -19987,7 +20085,7 @@
         <v>10.29764723777771</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -20008,7 +20106,7 @@
         <v>20.98466849327087</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>

</xml_diff>

<commit_message>
Updated C Cuda comparison table
</commit_message>
<xml_diff>
--- a/Summarized Trials.xlsx
+++ b/Summarized Trials.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e54ee0e16b764741/University/Fa2023/ECE 718 - Compiler Design for High Performance/Project/GemmCUDA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="696" documentId="13_ncr:1_{3C733FE7-E8A4-42C6-AC06-D019A0768725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C57D4296-893C-4E1D-9528-2A696B57576C}"/>
+  <xr:revisionPtr revIDLastSave="720" documentId="13_ncr:1_{3C733FE7-E8A4-42C6-AC06-D019A0768725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AEA7CA3-B7E8-4F39-8367-7D3945504BC9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Trials" sheetId="1" r:id="rId1"/>
     <sheet name="Context and Graphs" sheetId="2" r:id="rId2"/>
-    <sheet name="Trial 24 profiling" sheetId="3" r:id="rId3"/>
-    <sheet name="Trial 25 profiling" sheetId="4" r:id="rId4"/>
-    <sheet name="Trial 26 profiling" sheetId="6" r:id="rId5"/>
-    <sheet name="Trial 27 profiling" sheetId="5" r:id="rId6"/>
-    <sheet name="Trial 28 profiling" sheetId="7" r:id="rId7"/>
+    <sheet name="Trials Desc" sheetId="8" r:id="rId3"/>
+    <sheet name="Trial 24 profiling" sheetId="3" r:id="rId4"/>
+    <sheet name="Trial 25 profiling" sheetId="4" r:id="rId5"/>
+    <sheet name="Trial 26 profiling" sheetId="6" r:id="rId6"/>
+    <sheet name="Trial 27 profiling" sheetId="5" r:id="rId7"/>
+    <sheet name="Trial 28 profiling" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="465">
   <si>
     <t>Trial Name</t>
   </si>
@@ -1451,6 +1452,57 @@
   </si>
   <si>
     <t>GFLOPS/s</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>C (Boehm)</t>
+  </si>
+  <si>
+    <t>Trial #</t>
+  </si>
+  <si>
+    <t>Matrix Size</t>
+  </si>
+  <si>
+    <t>TILE_DIM</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>numba.cuda.cudadrv.driver.CudaAPIError: [700] Call to cuMemcpyDtoH results in UNKNOWN_CUDA_ERROR for shared memory access kernel</t>
+  </si>
+  <si>
+    <t>Works for vectorized kernel</t>
+  </si>
+  <si>
+    <t>Same as Trial 11, SM kernel profiled</t>
+  </si>
+  <si>
+    <t>Same as Trial 12, SM kernel profiled</t>
+  </si>
+  <si>
+    <t>Same as Trial 15, SM kernel profiled</t>
+  </si>
+  <si>
+    <t>Same as Trial 12, Vec kernel profiled</t>
+  </si>
+  <si>
+    <t>Same as Trial 18, Vec kernel profiled</t>
+  </si>
+  <si>
+    <t>Re-run for MKL and cuBLAS implementations</t>
+  </si>
+  <si>
+    <t>Re-run for MKL and cuBLAS implementations compare with CUDA kernels for curiosity's sake</t>
   </si>
 </sst>
 </file>
@@ -1877,7 +1929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2039,9 +2091,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17102,15 +17161,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2143125</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>2314575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>2219325</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17795,10 +17854,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -19186,10 +19241,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC22C78A-4AFB-42A7-860C-985947D40450}">
-  <dimension ref="A1:AG64"/>
+  <dimension ref="A1:AH64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AG12" sqref="AG12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B56" sqref="B56:I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19221,7 +19276,7 @@
     <col min="33" max="33" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>31</v>
       </c>
@@ -19285,14 +19340,14 @@
       <c r="AC1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AF1" s="71" t="s">
-        <v>446</v>
-      </c>
-      <c r="AG1" s="71" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG1" t="s">
+        <v>448</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>32</v>
       </c>
@@ -19363,14 +19418,17 @@
       <c r="AC2">
         <v>13.90225052833557</v>
       </c>
-      <c r="AF2" t="s">
-        <v>437</v>
-      </c>
-      <c r="AG2">
-        <v>1.7353403216161601E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AF2" s="41" t="s">
+        <v>446</v>
+      </c>
+      <c r="AG2" s="41" t="s">
+        <v>447</v>
+      </c>
+      <c r="AH2" s="41" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>64</v>
       </c>
@@ -19457,13 +19515,16 @@
         <v>13.905861854553221</v>
       </c>
       <c r="AF3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AG3">
-        <v>2.90926058637903E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+        <v>1.7353403216161601E-3</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>128</v>
       </c>
@@ -19550,13 +19611,16 @@
         <v>13.895543098449711</v>
       </c>
       <c r="AF4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AG4">
-        <v>0.84112840294118996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+        <v>2.90926058637903E-2</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>256</v>
       </c>
@@ -19643,13 +19707,16 @@
         <v>13.904776096343991</v>
       </c>
       <c r="AF5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AG5">
-        <v>17.738298566365501</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+        <v>0.84112840294118996</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>512</v>
       </c>
@@ -19736,13 +19803,16 @@
         <v>7.5108833312988281</v>
       </c>
       <c r="AF6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AG6">
-        <v>18.0753100449196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>17.738298566365501</v>
+      </c>
+      <c r="AH6">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>1024</v>
       </c>
@@ -19829,13 +19899,16 @@
         <v>7.5578842163085938</v>
       </c>
       <c r="AF7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AG7">
-        <v>29.0852894906571</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18.0753100449196</v>
+      </c>
+      <c r="AH7">
+        <v>1986.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>4096</v>
       </c>
@@ -19898,13 +19971,16 @@
         <v>7.5695807933807373</v>
       </c>
       <c r="AF8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AG8">
-        <v>18.298640440768601</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+        <v>29.0852894906571</v>
+      </c>
+      <c r="AH8">
+        <v>2980.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8192</v>
       </c>
@@ -19951,13 +20027,16 @@
         <v>7.6051571369171143</v>
       </c>
       <c r="AF9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AG9">
-        <v>30.6644762088862</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+        <v>18.298640440768601</v>
+      </c>
+      <c r="AH9">
+        <v>18237.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>16384</v>
       </c>
@@ -20004,13 +20083,16 @@
         <v>10.54792332649231</v>
       </c>
       <c r="AF10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AG10">
-        <v>170.55193128920101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+        <v>30.6644762088862</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="Y11" t="s">
         <v>24</v>
       </c>
@@ -20026,8 +20108,17 @@
       <c r="AC11">
         <v>10.497905492782589</v>
       </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AF11" t="s">
+        <v>445</v>
+      </c>
+      <c r="AG11">
+        <v>170.55193128920101</v>
+      </c>
+      <c r="AH11">
+        <v>23249.599999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="Y12" t="s">
         <v>25</v>
       </c>
@@ -20044,7 +20135,7 @@
         <v>21.146031141281131</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -20064,7 +20155,7 @@
         <v>10.286246299743651</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -20085,7 +20176,7 @@
         <v>10.29764723777771</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -20106,7 +20197,7 @@
         <v>20.98466849327087</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -20757,7 +20848,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="29" t="s">
         <v>233</v>
       </c>
@@ -21226,6 +21317,755 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1677DFF-6734-4837-B5F7-44C906E6ED0C}">
+  <dimension ref="A1:E43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="19.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="57.85546875" style="74" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
+        <v>450</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>451</v>
+      </c>
+      <c r="C1" s="71" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="71" t="s">
+        <v>452</v>
+      </c>
+      <c r="E1" s="72" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2">
+        <v>16</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>64</v>
+      </c>
+      <c r="C3" s="2">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2">
+        <v>16</v>
+      </c>
+      <c r="E3" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>128</v>
+      </c>
+      <c r="C4" s="2">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2">
+        <v>16</v>
+      </c>
+      <c r="E4" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>256</v>
+      </c>
+      <c r="C5" s="2">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2">
+        <v>16</v>
+      </c>
+      <c r="E5" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>512</v>
+      </c>
+      <c r="C6" s="2">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2">
+        <v>16</v>
+      </c>
+      <c r="E6" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1024</v>
+      </c>
+      <c r="C7" s="2">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2">
+        <v>16</v>
+      </c>
+      <c r="E7" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C8" s="2">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2">
+        <v>16</v>
+      </c>
+      <c r="E8" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4</v>
+      </c>
+      <c r="E9" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>16</v>
+      </c>
+      <c r="E11" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2">
+        <v>32</v>
+      </c>
+      <c r="E12" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C13" s="2">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4</v>
+      </c>
+      <c r="E13" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C14" s="2">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2">
+        <v>8</v>
+      </c>
+      <c r="E14" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C15" s="2">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2">
+        <v>16</v>
+      </c>
+      <c r="E15" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C16" s="2">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2">
+        <v>32</v>
+      </c>
+      <c r="E16" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="B17" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C17" s="2">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4</v>
+      </c>
+      <c r="E17" s="73" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="B18" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C18" s="2">
+        <v>16</v>
+      </c>
+      <c r="D18" s="2">
+        <v>8</v>
+      </c>
+      <c r="E18" s="73" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C19" s="2">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2">
+        <v>16</v>
+      </c>
+      <c r="E19" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C20" s="2">
+        <v>16</v>
+      </c>
+      <c r="D20" s="2">
+        <v>32</v>
+      </c>
+      <c r="E20" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="B21" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C21" s="2">
+        <v>32</v>
+      </c>
+      <c r="D21" s="2">
+        <v>4</v>
+      </c>
+      <c r="E21" s="73" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="B22" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C22" s="2">
+        <v>32</v>
+      </c>
+      <c r="D22" s="2">
+        <v>8</v>
+      </c>
+      <c r="E22" s="73" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="B23" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C23" s="2">
+        <v>32</v>
+      </c>
+      <c r="D23" s="2">
+        <v>16</v>
+      </c>
+      <c r="E23" s="73" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>18</v>
+      </c>
+      <c r="B24" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C24" s="2">
+        <v>32</v>
+      </c>
+      <c r="D24" s="2">
+        <v>32</v>
+      </c>
+      <c r="E24" s="73" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>19</v>
+      </c>
+      <c r="B25" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C25" s="2">
+        <v>16</v>
+      </c>
+      <c r="D25" s="2">
+        <v>4</v>
+      </c>
+      <c r="E25" s="73" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>20</v>
+      </c>
+      <c r="B26" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C26" s="2">
+        <v>16</v>
+      </c>
+      <c r="D26" s="2">
+        <v>8</v>
+      </c>
+      <c r="E26" s="73" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>21</v>
+      </c>
+      <c r="B27" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C27" s="2">
+        <v>32</v>
+      </c>
+      <c r="D27" s="2">
+        <v>4</v>
+      </c>
+      <c r="E27" s="73" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>22</v>
+      </c>
+      <c r="B28" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C28" s="2">
+        <v>32</v>
+      </c>
+      <c r="D28" s="2">
+        <v>8</v>
+      </c>
+      <c r="E28" s="73" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>23</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C29" s="2">
+        <v>32</v>
+      </c>
+      <c r="D29" s="2">
+        <v>16</v>
+      </c>
+      <c r="E29" s="73" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>24</v>
+      </c>
+      <c r="B30" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C30" s="2">
+        <v>4</v>
+      </c>
+      <c r="D30" s="2">
+        <v>32</v>
+      </c>
+      <c r="E30" s="73" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>25</v>
+      </c>
+      <c r="B31" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C31" s="2">
+        <v>8</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4</v>
+      </c>
+      <c r="E31" s="73" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>26</v>
+      </c>
+      <c r="B32" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C32" s="2">
+        <v>8</v>
+      </c>
+      <c r="D32" s="2">
+        <v>32</v>
+      </c>
+      <c r="E32" s="73" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>27</v>
+      </c>
+      <c r="B33" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C33" s="2">
+        <v>8</v>
+      </c>
+      <c r="D33" s="2">
+        <v>4</v>
+      </c>
+      <c r="E33" s="73" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>28</v>
+      </c>
+      <c r="B34" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C34" s="2">
+        <v>32</v>
+      </c>
+      <c r="D34" s="2">
+        <v>32</v>
+      </c>
+      <c r="E34" s="73" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>30</v>
+      </c>
+      <c r="B35" s="2">
+        <v>32</v>
+      </c>
+      <c r="C35" s="2">
+        <v>16</v>
+      </c>
+      <c r="D35" s="2">
+        <v>16</v>
+      </c>
+      <c r="E35" s="73" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>31</v>
+      </c>
+      <c r="B36" s="2">
+        <v>64</v>
+      </c>
+      <c r="C36" s="2">
+        <v>16</v>
+      </c>
+      <c r="D36" s="2">
+        <v>16</v>
+      </c>
+      <c r="E36" s="73" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>32</v>
+      </c>
+      <c r="B37" s="2">
+        <v>128</v>
+      </c>
+      <c r="C37" s="2">
+        <v>16</v>
+      </c>
+      <c r="D37" s="2">
+        <v>16</v>
+      </c>
+      <c r="E37" s="73" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>33</v>
+      </c>
+      <c r="B38" s="2">
+        <v>256</v>
+      </c>
+      <c r="C38" s="2">
+        <v>16</v>
+      </c>
+      <c r="D38" s="2">
+        <v>16</v>
+      </c>
+      <c r="E38" s="73" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>34</v>
+      </c>
+      <c r="B39" s="2">
+        <v>512</v>
+      </c>
+      <c r="C39" s="2">
+        <v>16</v>
+      </c>
+      <c r="D39" s="2">
+        <v>16</v>
+      </c>
+      <c r="E39" s="73" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>35</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1024</v>
+      </c>
+      <c r="C40" s="2">
+        <v>16</v>
+      </c>
+      <c r="D40" s="2">
+        <v>16</v>
+      </c>
+      <c r="E40" s="73" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>36</v>
+      </c>
+      <c r="B41" s="2">
+        <v>4096</v>
+      </c>
+      <c r="C41" s="2">
+        <v>16</v>
+      </c>
+      <c r="D41" s="2">
+        <v>16</v>
+      </c>
+      <c r="E41" s="73" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>37</v>
+      </c>
+      <c r="B42" s="2">
+        <v>8192</v>
+      </c>
+      <c r="C42" s="2">
+        <v>16</v>
+      </c>
+      <c r="D42" s="2">
+        <v>16</v>
+      </c>
+      <c r="E42" s="73" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>38</v>
+      </c>
+      <c r="B43" s="2">
+        <v>16384</v>
+      </c>
+      <c r="C43" s="2">
+        <v>16</v>
+      </c>
+      <c r="D43" s="2">
+        <v>16</v>
+      </c>
+      <c r="E43" s="73" t="s">
+        <v>464</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E792B270-628C-4C5A-98ED-E54E52F50D15}">
   <dimension ref="A1:I33"/>
   <sheetViews>
@@ -21923,7 +22763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9FEAAE-796E-4BB7-93D4-9B8A8872AF3E}">
   <dimension ref="A1:I33"/>
   <sheetViews>
@@ -22618,7 +23458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B6343C-3FF5-42EB-B10B-FD4A16692DF7}">
   <dimension ref="A1:I33"/>
   <sheetViews>
@@ -23315,7 +24155,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBFB017B-43D6-47D7-9217-AA6ACC8F4FD6}">
   <dimension ref="A1:T33"/>
   <sheetViews>
@@ -24130,7 +24970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82141C89-A3E5-4070-B989-19AC98B4C496}">
   <dimension ref="A1:I33"/>
   <sheetViews>

</xml_diff>